<commit_message>
Updated stats page, monthly reset message. Also made no rows in cornucopia result in a total loss.
</commit_message>
<xml_diff>
--- a/cornucopia_rates.xlsx
+++ b/cornucopia_rates.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jckaw\GitHub\corn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D633D0C2-FE02-4379-A861-627C14842A35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF404712-1888-4E93-B03D-0520D58963DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11200" yWindow="390" windowWidth="18630" windowHeight="14670" xr2:uid="{B8E97D5F-91D4-4475-8CF4-6E9967CD7B11}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{B8E97D5F-91D4-4475-8CF4-6E9967CD7B11}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -125,7 +126,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -280,11 +281,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -305,6 +317,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FAF9209-FB9E-4F97-BAE4-B558D985DC4D}">
-  <dimension ref="B2:K41"/>
+  <dimension ref="B2:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="97" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -634,15 +647,16 @@
     <col min="7" max="7" width="13.36328125" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
     <col min="11" max="11" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="10">
         <f>SUM(E8:E39)</f>
-        <v>10077696</v>
+        <v>1953125</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>8</v>
@@ -651,13 +665,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="10" cm="1">
         <f t="array" ref="C3">SUM(E8:E39*H8:H39)/C2</f>
-        <v>1.1981481481481482</v>
+        <v>1.2943999999999998</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>1</v>
@@ -666,7 +680,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
@@ -674,15 +688,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="E5" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
@@ -705,7 +719,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" s="13">
         <v>0</v>
       </c>
@@ -715,12 +729,12 @@
       <c r="D8" s="12">
         <v>0</v>
       </c>
-      <c r="E8" s="13">
-        <v>2506596</v>
+      <c r="E8" s="20">
+        <v>596704</v>
       </c>
       <c r="F8" s="16">
         <f>E8/$C$2</f>
-        <v>0.24872709000152415</v>
+        <v>0.30551244799999999</v>
       </c>
       <c r="G8" s="14">
         <f>B8*$F$3+C8*$F$4+D8*$F$5</f>
@@ -731,7 +745,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" s="14">
         <v>0</v>
       </c>
@@ -741,23 +755,23 @@
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="E9" s="14">
-        <v>2453814</v>
+      <c r="E9" s="11">
+        <v>367632</v>
       </c>
       <c r="F9" s="17">
         <f t="shared" ref="F9:F39" si="0">E9/$C$2</f>
-        <v>0.24348958333333334</v>
+        <v>0.188227584</v>
       </c>
       <c r="G9" s="14">
         <f t="shared" ref="G9:G39" si="1">B9*$F$3+C9*$F$4+D9*$F$5</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H9" s="4">
-        <f t="shared" ref="H9:H39" si="2">0.2+G9*1.1</f>
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+        <f t="shared" ref="H9:H39" si="2">0.2+G9*0.9</f>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" s="14">
         <v>0</v>
       </c>
@@ -767,23 +781,23 @@
       <c r="D10">
         <v>2</v>
       </c>
-      <c r="E10" s="14">
-        <v>1377810</v>
+      <c r="E10" s="11">
+        <v>137664</v>
       </c>
       <c r="F10" s="17">
         <f t="shared" si="0"/>
-        <v>0.13671875</v>
+        <v>7.0483967999999994E-2</v>
       </c>
       <c r="G10" s="14">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10" s="4">
         <f t="shared" si="2"/>
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11" s="14">
         <v>0</v>
       </c>
@@ -793,23 +807,23 @@
       <c r="D11">
         <v>3</v>
       </c>
-      <c r="E11" s="14">
-        <v>669222</v>
+      <c r="E11" s="11">
+        <v>48384</v>
       </c>
       <c r="F11" s="17">
         <f t="shared" si="0"/>
-        <v>6.640625E-2</v>
+        <v>2.4772608000000002E-2</v>
       </c>
       <c r="G11" s="14">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="H11" s="4">
         <f t="shared" si="2"/>
-        <v>1.85</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
+        <v>2.9000000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B12" s="14">
         <v>0</v>
       </c>
@@ -819,24 +833,23 @@
       <c r="D12">
         <v>4</v>
       </c>
-      <c r="E12" s="14">
-        <v>255879</v>
+      <c r="E12" s="11">
+        <v>14592</v>
       </c>
       <c r="F12" s="17">
         <f t="shared" si="0"/>
-        <v>2.5390625E-2</v>
+        <v>7.4711040000000001E-3</v>
       </c>
       <c r="G12" s="14">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H12" s="4">
         <f t="shared" si="2"/>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
+        <v>3.8000000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B13" s="14">
         <v>0</v>
       </c>
@@ -846,23 +859,23 @@
       <c r="D13">
         <v>5</v>
       </c>
-      <c r="E13" s="14">
-        <v>118098</v>
+      <c r="E13" s="11">
+        <v>5376</v>
       </c>
       <c r="F13" s="17">
         <f t="shared" si="0"/>
-        <v>1.171875E-2</v>
+        <v>2.7525119999999999E-3</v>
       </c>
       <c r="G13" s="14">
         <f t="shared" si="1"/>
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="H13" s="4">
         <f t="shared" si="2"/>
-        <v>2.95</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B14" s="14">
         <v>0</v>
       </c>
@@ -872,23 +885,23 @@
       <c r="D14">
         <v>6</v>
       </c>
-      <c r="E14" s="14">
-        <v>78732</v>
+      <c r="E14" s="11">
+        <v>3072</v>
       </c>
       <c r="F14" s="17">
         <f t="shared" si="0"/>
-        <v>7.8125E-3</v>
+        <v>1.572864E-3</v>
       </c>
       <c r="G14" s="14">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H14" s="4">
         <f t="shared" si="2"/>
-        <v>3.5000000000000004</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
+        <v>5.6000000000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B15" s="14">
         <v>0</v>
       </c>
@@ -898,23 +911,23 @@
       <c r="D15">
         <v>8</v>
       </c>
-      <c r="E15" s="14">
-        <v>19683</v>
+      <c r="E15" s="11">
+        <v>512</v>
       </c>
       <c r="F15" s="17">
         <f t="shared" si="0"/>
-        <v>1.953125E-3</v>
+        <v>2.6214400000000002E-4</v>
       </c>
       <c r="G15" s="14">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H15" s="4">
         <f t="shared" si="2"/>
-        <v>4.6000000000000005</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B16" s="14">
         <v>0</v>
       </c>
@@ -924,12 +937,12 @@
       <c r="D16">
         <v>0</v>
       </c>
-      <c r="E16" s="14">
-        <v>1231616</v>
+      <c r="E16" s="11">
+        <v>367632</v>
       </c>
       <c r="F16" s="17">
         <f t="shared" si="0"/>
-        <v>0.12221206116953716</v>
+        <v>0.188227584</v>
       </c>
       <c r="G16" s="14">
         <f t="shared" si="1"/>
@@ -937,7 +950,7 @@
       </c>
       <c r="H16" s="4">
         <f t="shared" si="2"/>
-        <v>1.3</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.35">
@@ -950,20 +963,20 @@
       <c r="D17">
         <v>1</v>
       </c>
-      <c r="E17" s="14">
-        <v>466560</v>
+      <c r="E17" s="11">
+        <v>82944</v>
       </c>
       <c r="F17" s="17">
         <f t="shared" si="0"/>
-        <v>4.6296296296296294E-2</v>
+        <v>4.2467327999999999E-2</v>
       </c>
       <c r="G17" s="14">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="H17" s="4">
         <f t="shared" si="2"/>
-        <v>1.85</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.35">
@@ -976,20 +989,20 @@
       <c r="D18">
         <v>2</v>
       </c>
-      <c r="E18" s="14">
-        <v>34992</v>
+      <c r="E18" s="11">
+        <v>3072</v>
       </c>
       <c r="F18" s="17">
         <f t="shared" si="0"/>
-        <v>3.472222222222222E-3</v>
+        <v>1.572864E-3</v>
       </c>
       <c r="G18" s="14">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H18" s="4">
         <f t="shared" si="2"/>
-        <v>2.4000000000000004</v>
+        <v>2.9000000000000004</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.35">
@@ -1002,12 +1015,12 @@
       <c r="D19">
         <v>0</v>
       </c>
-      <c r="E19" s="14">
-        <v>366080</v>
+      <c r="E19" s="11">
+        <v>137664</v>
       </c>
       <c r="F19" s="17">
         <f t="shared" si="0"/>
-        <v>3.6325763349082968E-2</v>
+        <v>7.0483967999999994E-2</v>
       </c>
       <c r="G19" s="14">
         <f t="shared" si="1"/>
@@ -1015,7 +1028,7 @@
       </c>
       <c r="H19" s="4">
         <f t="shared" si="2"/>
-        <v>2.4000000000000004</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.35">
@@ -1028,20 +1041,20 @@
       <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" s="14">
-        <v>10368</v>
+      <c r="E20" s="11">
+        <v>3072</v>
       </c>
       <c r="F20" s="17">
         <f t="shared" si="0"/>
-        <v>1.02880658436214E-3</v>
+        <v>1.572864E-3</v>
       </c>
       <c r="G20" s="14">
         <f t="shared" si="1"/>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="H20" s="4">
         <f t="shared" si="2"/>
-        <v>2.95</v>
+        <v>2.9000000000000004</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.35">
@@ -1054,12 +1067,12 @@
       <c r="D21">
         <v>0</v>
       </c>
-      <c r="E21" s="14">
-        <v>102400</v>
+      <c r="E21" s="11">
+        <v>48384</v>
       </c>
       <c r="F21" s="17">
         <f t="shared" si="0"/>
-        <v>1.0161052685058172E-2</v>
+        <v>2.4772608000000002E-2</v>
       </c>
       <c r="G21" s="14">
         <f t="shared" si="1"/>
@@ -1067,7 +1080,7 @@
       </c>
       <c r="H21" s="4">
         <f t="shared" si="2"/>
-        <v>3.5000000000000004</v>
+        <v>2.9000000000000004</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.35">
@@ -1080,12 +1093,12 @@
       <c r="D22">
         <v>0</v>
       </c>
-      <c r="E22" s="14">
-        <v>25600</v>
+      <c r="E22" s="11">
+        <v>14592</v>
       </c>
       <c r="F22" s="17">
         <f t="shared" si="0"/>
-        <v>2.540263171264543E-3</v>
+        <v>7.4711040000000001E-3</v>
       </c>
       <c r="G22" s="14">
         <f t="shared" si="1"/>
@@ -1093,7 +1106,7 @@
       </c>
       <c r="H22" s="4">
         <f t="shared" si="2"/>
-        <v>4.6000000000000005</v>
+        <v>3.8000000000000003</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.35">
@@ -1106,12 +1119,12 @@
       <c r="D23">
         <v>0</v>
       </c>
-      <c r="E23" s="14">
-        <v>8192</v>
+      <c r="E23" s="11">
+        <v>5376</v>
       </c>
       <c r="F23" s="17">
         <f t="shared" si="0"/>
-        <v>8.1288421480465371E-4</v>
+        <v>2.7525119999999999E-3</v>
       </c>
       <c r="G23" s="14">
         <f t="shared" si="1"/>
@@ -1119,7 +1132,7 @@
       </c>
       <c r="H23" s="4">
         <f t="shared" si="2"/>
-        <v>5.7</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.35">
@@ -1132,12 +1145,12 @@
       <c r="D24">
         <v>0</v>
       </c>
-      <c r="E24" s="14">
-        <v>4096</v>
+      <c r="E24" s="11">
+        <v>3072</v>
       </c>
       <c r="F24" s="17">
         <f t="shared" si="0"/>
-        <v>4.0644210740232686E-4</v>
+        <v>1.572864E-3</v>
       </c>
       <c r="G24" s="14">
         <f t="shared" si="1"/>
@@ -1145,7 +1158,7 @@
       </c>
       <c r="H24" s="4">
         <f t="shared" si="2"/>
-        <v>6.8000000000000007</v>
+        <v>5.6000000000000005</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.35">
@@ -1158,12 +1171,12 @@
       <c r="D25">
         <v>0</v>
       </c>
-      <c r="E25" s="14">
+      <c r="E25" s="11">
         <v>512</v>
       </c>
       <c r="F25" s="17">
         <f t="shared" si="0"/>
-        <v>5.0805263425290857E-5</v>
+        <v>2.6214400000000002E-4</v>
       </c>
       <c r="G25" s="14">
         <f t="shared" si="1"/>
@@ -1171,7 +1184,7 @@
       </c>
       <c r="H25" s="4">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.35">
@@ -1184,12 +1197,12 @@
       <c r="D26">
         <v>0</v>
       </c>
-      <c r="E26" s="14">
-        <v>242050</v>
+      <c r="E26" s="11">
+        <v>80384</v>
       </c>
       <c r="F26" s="17">
         <f t="shared" si="0"/>
-        <v>2.4018386742366508E-2</v>
+        <v>4.1156607999999997E-2</v>
       </c>
       <c r="G26" s="14">
         <f t="shared" si="1"/>
@@ -1197,7 +1210,7 @@
       </c>
       <c r="H26" s="4">
         <f t="shared" si="2"/>
-        <v>3.5000000000000004</v>
+        <v>2.9000000000000004</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.35">
@@ -1210,20 +1223,20 @@
       <c r="D27">
         <v>1</v>
       </c>
-      <c r="E27" s="14">
-        <v>58320</v>
+      <c r="E27" s="11">
+        <v>10368</v>
       </c>
       <c r="F27" s="17">
         <f t="shared" si="0"/>
-        <v>5.7870370370370367E-3</v>
+        <v>5.3084159999999998E-3</v>
       </c>
       <c r="G27" s="14">
         <f t="shared" si="1"/>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="H27" s="4">
         <f t="shared" si="2"/>
-        <v>4.0500000000000007</v>
+        <v>3.8000000000000003</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.35">
@@ -1236,20 +1249,20 @@
       <c r="D28">
         <v>2</v>
       </c>
-      <c r="E28" s="14">
-        <v>4374</v>
+      <c r="E28" s="11">
+        <v>384</v>
       </c>
       <c r="F28" s="17">
         <f t="shared" si="0"/>
-        <v>4.3402777777777775E-4</v>
+        <v>1.96608E-4</v>
       </c>
       <c r="G28" s="14">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H28" s="4">
         <f t="shared" si="2"/>
-        <v>4.6000000000000005</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.35">
@@ -1262,12 +1275,12 @@
       <c r="D29">
         <v>0</v>
       </c>
-      <c r="E29" s="14">
-        <v>17280</v>
+      <c r="E29" s="11">
+        <v>10368</v>
       </c>
       <c r="F29" s="17">
         <f t="shared" si="0"/>
-        <v>1.7146776406035665E-3</v>
+        <v>5.3084159999999998E-3</v>
       </c>
       <c r="G29" s="14">
         <f t="shared" si="1"/>
@@ -1275,7 +1288,7 @@
       </c>
       <c r="H29" s="4">
         <f t="shared" si="2"/>
-        <v>4.6000000000000005</v>
+        <v>3.8000000000000003</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.35">
@@ -1288,20 +1301,20 @@
       <c r="D30">
         <v>1</v>
       </c>
-      <c r="E30" s="14">
-        <v>2592</v>
+      <c r="E30" s="11">
+        <v>768</v>
       </c>
       <c r="F30" s="17">
         <f t="shared" si="0"/>
-        <v>2.57201646090535E-4</v>
+        <v>3.93216E-4</v>
       </c>
       <c r="G30" s="14">
         <f t="shared" si="1"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="H30" s="4">
         <f t="shared" si="2"/>
-        <v>5.15</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.35">
@@ -1314,12 +1327,12 @@
       <c r="D31">
         <v>0</v>
       </c>
-      <c r="E31" s="14">
+      <c r="E31" s="11">
         <v>384</v>
       </c>
       <c r="F31" s="17">
         <f t="shared" si="0"/>
-        <v>3.8103947568968146E-5</v>
+        <v>1.96608E-4</v>
       </c>
       <c r="G31" s="14">
         <f t="shared" si="1"/>
@@ -1327,7 +1340,7 @@
       </c>
       <c r="H31" s="4">
         <f t="shared" si="2"/>
-        <v>5.7</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.35">
@@ -1340,12 +1353,12 @@
       <c r="D32">
         <v>0</v>
       </c>
-      <c r="E32" s="14">
-        <v>19390</v>
+      <c r="E32" s="11">
+        <v>8544</v>
       </c>
       <c r="F32" s="17">
         <f t="shared" si="0"/>
-        <v>1.9240508941726364E-3</v>
+        <v>4.3745279999999999E-3</v>
       </c>
       <c r="G32" s="14">
         <f t="shared" si="1"/>
@@ -1353,7 +1366,7 @@
       </c>
       <c r="H32" s="4">
         <f t="shared" si="2"/>
-        <v>6.8000000000000007</v>
+        <v>5.6000000000000005</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.35">
@@ -1366,20 +1379,20 @@
       <c r="D33">
         <v>1</v>
       </c>
-      <c r="E33" s="14">
-        <v>162</v>
+      <c r="E33" s="11">
+        <v>48</v>
       </c>
       <c r="F33" s="17">
         <f t="shared" si="0"/>
-        <v>1.6075102880658438E-5</v>
+        <v>2.4576E-5</v>
       </c>
       <c r="G33" s="14">
         <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="H33" s="4">
+        <f t="shared" si="2"/>
         <v>6.5</v>
-      </c>
-      <c r="H33" s="4">
-        <f t="shared" si="2"/>
-        <v>7.3500000000000005</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.35">
@@ -1392,12 +1405,12 @@
       <c r="D34">
         <v>0</v>
       </c>
-      <c r="E34" s="14">
+      <c r="E34" s="11">
         <v>48</v>
       </c>
       <c r="F34" s="17">
         <f t="shared" si="0"/>
-        <v>4.7629934461210183E-6</v>
+        <v>2.4576E-5</v>
       </c>
       <c r="G34" s="14">
         <f t="shared" si="1"/>
@@ -1405,7 +1418,7 @@
       </c>
       <c r="H34" s="4">
         <f t="shared" si="2"/>
-        <v>7.9000000000000012</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.35">
@@ -1418,12 +1431,12 @@
       <c r="D35">
         <v>0</v>
       </c>
-      <c r="E35" s="14">
-        <v>2450</v>
+      <c r="E35" s="11">
+        <v>1312</v>
       </c>
       <c r="F35" s="17">
         <f t="shared" si="0"/>
-        <v>2.4311112381242696E-4</v>
+        <v>6.7174400000000005E-4</v>
       </c>
       <c r="G35" s="14">
         <f t="shared" si="1"/>
@@ -1431,7 +1444,7 @@
       </c>
       <c r="H35" s="4">
         <f t="shared" si="2"/>
-        <v>10.1</v>
+        <v>8.2999999999999989</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.35">
@@ -1444,12 +1457,12 @@
       <c r="D36">
         <v>0</v>
       </c>
-      <c r="E36" s="14">
-        <v>305</v>
+      <c r="E36" s="11">
+        <v>196</v>
       </c>
       <c r="F36" s="17">
         <f t="shared" si="0"/>
-        <v>3.0264854188893968E-5</v>
+        <v>1.00352E-4</v>
       </c>
       <c r="G36" s="14">
         <f t="shared" si="1"/>
@@ -1457,7 +1470,7 @@
       </c>
       <c r="H36" s="4">
         <f t="shared" si="2"/>
-        <v>13.4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.35">
@@ -1470,12 +1483,12 @@
       <c r="D37">
         <v>0</v>
       </c>
-      <c r="E37" s="14">
-        <v>70</v>
+      <c r="E37" s="11">
+        <v>48</v>
       </c>
       <c r="F37" s="17">
         <f t="shared" si="0"/>
-        <v>6.9460321089264847E-6</v>
+        <v>2.4576E-5</v>
       </c>
       <c r="G37" s="14">
         <f t="shared" si="1"/>
@@ -1483,7 +1496,7 @@
       </c>
       <c r="H37" s="4">
         <f t="shared" si="2"/>
-        <v>16.7</v>
+        <v>13.7</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.35">
@@ -1496,12 +1509,12 @@
       <c r="D38">
         <v>0</v>
       </c>
-      <c r="E38" s="14">
-        <v>20</v>
+      <c r="E38" s="11">
+        <v>16</v>
       </c>
       <c r="F38" s="17">
         <f t="shared" si="0"/>
-        <v>1.9845806025504242E-6</v>
+        <v>8.1920000000000005E-6</v>
       </c>
       <c r="G38" s="14">
         <f t="shared" si="1"/>
@@ -1509,7 +1522,7 @@
       </c>
       <c r="H38" s="4">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>16.399999999999999</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.35">
@@ -1522,12 +1535,12 @@
       <c r="D39" s="7">
         <v>0</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E39" s="8">
         <v>1</v>
       </c>
       <c r="F39" s="18">
         <f t="shared" si="0"/>
-        <v>9.9229030127521205E-8</v>
+        <v>5.1200000000000003E-7</v>
       </c>
       <c r="G39" s="6">
         <f t="shared" si="1"/>
@@ -1535,7 +1548,7 @@
       </c>
       <c r="H39" s="5">
         <f t="shared" si="2"/>
-        <v>26.6</v>
+        <v>21.8</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.35">
@@ -1543,6 +1556,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>